<commit_message>
ultimo arreglo a progress table
</commit_message>
<xml_diff>
--- a/Progress Table.xlsx
+++ b/Progress Table.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sis Comp\Ingeniería de software\Proyecto\"/>
@@ -18,7 +18,7 @@
     <sheet name="Burn Down Chart" sheetId="4" r:id="rId4"/>
     <sheet name="Burn Down Graph" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="196">
   <si>
     <t>System Requeriments</t>
   </si>
@@ -604,12 +604,24 @@
   </si>
   <si>
     <t>Yo como usuario quiero agregar un tratamiento médico, entonces debo llevar un formulario con la información del tratamiento.</t>
+  </si>
+  <si>
+    <t>Programa de escritorio</t>
+  </si>
+  <si>
+    <t>Programa en linea</t>
+  </si>
+  <si>
+    <t>Edgar, Julissa, Eduardo</t>
+  </si>
+  <si>
+    <t>Andrés, Pablo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -757,7 +769,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -873,32 +885,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -917,21 +903,6 @@
         <color indexed="64"/>
       </top>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -989,7 +960,29 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -1001,6 +994,34 @@
         <color indexed="64"/>
       </right>
       <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1008,9 +1029,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -1021,8 +1040,84 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom/>
@@ -1033,8 +1128,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1043,10 +1140,25 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1062,90 +1174,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1154,7 +1183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="157">
+  <cellXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1262,7 +1291,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1286,29 +1315,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1316,23 +1331,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1340,46 +1346,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="26" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1413,73 +1419,73 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="31" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1494,10 +1500,53 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1551,7 +1600,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -1596,7 +1645,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1698,9 +1746,8 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+            <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -1720,33 +1767,33 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>'Burn Down Chart'!$E$19:$M$19</c:f>
+              <c:f>'Burn Down Chart'!$E$21:$M$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>165</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>131</c:v>
+                  <c:v>166</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>119</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>119</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>79</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79</c:v>
+                  <c:v>114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>56</c:v>
+                  <c:v>89</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>61</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -1755,7 +1802,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-187A-48AB-B3ED-524699FA1603}"/>
             </c:ext>
@@ -1820,7 +1867,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1938,7 +1984,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2610,7 +2655,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{9E18B2AE-1F19-4710-8DE8-C20AFC1944B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E18B2AE-1F19-4710-8DE8-C20AFC1944B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2932,7 +2977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AB58"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8:O15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2997,8 +3044,8 @@
       <c r="O3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="Q3" s="120"/>
-      <c r="R3" s="117"/>
+      <c r="Q3" s="111"/>
+      <c r="R3" s="108"/>
       <c r="S3" s="25"/>
       <c r="T3" s="25"/>
       <c r="U3" s="25"/>
@@ -3011,34 +3058,34 @@
       <c r="AB3" s="25"/>
     </row>
     <row r="4" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B4" s="137" t="s">
+      <c r="B4" s="128" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="138" t="s">
+      <c r="C4" s="129" t="s">
         <v>30</v>
       </c>
-      <c r="D4" s="139" t="s">
+      <c r="D4" s="130" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="138" t="s">
+      <c r="E4" s="129" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="140" t="s">
+      <c r="F4" s="131" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="141" t="s">
+      <c r="G4" s="132" t="s">
         <v>26</v>
       </c>
-      <c r="H4" s="139" t="s">
+      <c r="H4" s="130" t="s">
         <v>34</v>
       </c>
-      <c r="I4" s="138" t="s">
+      <c r="I4" s="129" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="139" t="s">
+      <c r="J4" s="130" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="142" t="s">
+      <c r="K4" s="133" t="s">
         <v>19</v>
       </c>
       <c r="M4" s="3" t="s">
@@ -3064,16 +3111,16 @@
       <c r="AB4" s="25"/>
     </row>
     <row r="5" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B5" s="129"/>
-      <c r="C5" s="130"/>
-      <c r="D5" s="131"/>
-      <c r="E5" s="130"/>
-      <c r="F5" s="132"/>
-      <c r="G5" s="150"/>
-      <c r="H5" s="131"/>
-      <c r="I5" s="130"/>
-      <c r="J5" s="131"/>
-      <c r="K5" s="136"/>
+      <c r="B5" s="120"/>
+      <c r="C5" s="121"/>
+      <c r="D5" s="122"/>
+      <c r="E5" s="121"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="141"/>
+      <c r="H5" s="122"/>
+      <c r="I5" s="121"/>
+      <c r="J5" s="122"/>
+      <c r="K5" s="127"/>
       <c r="M5" s="20" t="s">
         <v>70</v>
       </c>
@@ -3097,34 +3144,34 @@
       <c r="AB5" s="25"/>
     </row>
     <row r="6" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="116" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="126" t="s">
+      <c r="C6" s="117" t="s">
         <v>31</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="126" t="s">
+      <c r="E6" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="F6" s="127" t="s">
+      <c r="F6" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="143" t="s">
+      <c r="G6" s="134" t="s">
         <v>23</v>
       </c>
       <c r="H6" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="126" t="s">
+      <c r="I6" s="117" t="s">
         <v>26</v>
       </c>
       <c r="J6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K6" s="128" t="s">
+      <c r="K6" s="119" t="s">
         <v>19</v>
       </c>
       <c r="M6" s="5" t="s">
@@ -3142,34 +3189,34 @@
       <c r="T6" s="25"/>
       <c r="U6" s="25"/>
       <c r="V6" s="25"/>
-      <c r="W6" s="120"/>
-      <c r="X6" s="117"/>
+      <c r="W6" s="111"/>
+      <c r="X6" s="108"/>
       <c r="Y6" s="25"/>
       <c r="Z6" s="25"/>
       <c r="AA6" s="25"/>
       <c r="AB6" s="25"/>
     </row>
     <row r="7" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="125"/>
-      <c r="C7" s="126"/>
+      <c r="B7" s="116"/>
+      <c r="C7" s="117"/>
       <c r="D7" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="E7" s="126" t="s">
+      <c r="E7" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="F7" s="127" t="s">
+      <c r="F7" s="118" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="143"/>
+      <c r="G7" s="134"/>
       <c r="H7" s="11"/>
-      <c r="I7" s="126" t="s">
+      <c r="I7" s="117" t="s">
         <v>27</v>
       </c>
       <c r="J7" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="128" t="s">
+      <c r="K7" s="119" t="s">
         <v>19</v>
       </c>
       <c r="Q7" s="43"/>
@@ -3186,16 +3233,16 @@
       <c r="AB7" s="25"/>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="129"/>
-      <c r="C8" s="130"/>
-      <c r="D8" s="131"/>
-      <c r="E8" s="130"/>
-      <c r="F8" s="132"/>
-      <c r="G8" s="133"/>
-      <c r="H8" s="134"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="131"/>
-      <c r="K8" s="136"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="121"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="121"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="126"/>
+      <c r="J8" s="122"/>
+      <c r="K8" s="127"/>
       <c r="M8" s="12"/>
       <c r="N8" s="14" t="s">
         <v>7</v>
@@ -3215,34 +3262,34 @@
       <c r="AB8" s="25"/>
     </row>
     <row r="9" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="125" t="s">
+      <c r="B9" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="126" t="s">
+      <c r="C9" s="117" t="s">
         <v>32</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="126" t="s">
+      <c r="E9" s="117" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="127" t="s">
+      <c r="F9" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="143" t="s">
+      <c r="G9" s="134" t="s">
         <v>23</v>
       </c>
       <c r="H9" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="126" t="s">
+      <c r="I9" s="117" t="s">
         <v>24</v>
       </c>
       <c r="J9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="128" t="s">
+      <c r="K9" s="119" t="s">
         <v>19</v>
       </c>
       <c r="M9" s="36" t="s">
@@ -3252,8 +3299,8 @@
       <c r="O9" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="Q9" s="120"/>
-      <c r="R9" s="117"/>
+      <c r="Q9" s="111"/>
+      <c r="R9" s="108"/>
       <c r="S9" s="25"/>
       <c r="T9" s="25"/>
       <c r="U9" s="25"/>
@@ -3266,16 +3313,16 @@
       <c r="AB9" s="25"/>
     </row>
     <row r="10" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B10" s="129"/>
-      <c r="C10" s="130"/>
-      <c r="D10" s="131"/>
-      <c r="E10" s="130"/>
-      <c r="F10" s="132"/>
-      <c r="G10" s="150"/>
-      <c r="H10" s="131"/>
-      <c r="I10" s="130"/>
-      <c r="J10" s="131"/>
-      <c r="K10" s="136"/>
+      <c r="B10" s="120"/>
+      <c r="C10" s="121"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="123"/>
+      <c r="G10" s="141"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="121"/>
+      <c r="J10" s="122"/>
+      <c r="K10" s="127"/>
       <c r="M10" s="3" t="s">
         <v>69</v>
       </c>
@@ -3299,34 +3346,34 @@
       <c r="AB10" s="25"/>
     </row>
     <row r="11" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B11" s="125" t="s">
+      <c r="B11" s="116" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="126" t="s">
+      <c r="C11" s="117" t="s">
         <v>33</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="126" t="s">
+      <c r="E11" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="F11" s="127" t="s">
+      <c r="F11" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="143" t="s">
+      <c r="G11" s="134" t="s">
         <v>23</v>
       </c>
       <c r="H11" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="126" t="s">
+      <c r="I11" s="117" t="s">
         <v>26</v>
       </c>
       <c r="J11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="128" t="s">
+      <c r="K11" s="119" t="s">
         <v>19</v>
       </c>
       <c r="M11" s="20" t="s">
@@ -3352,22 +3399,22 @@
       <c r="AB11" s="25"/>
     </row>
     <row r="12" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B12" s="125"/>
-      <c r="C12" s="126"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="117"/>
       <c r="D12" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="126" t="s">
+      <c r="E12" s="117" t="s">
         <v>14</v>
       </c>
-      <c r="F12" s="127" t="s">
+      <c r="F12" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="150"/>
-      <c r="H12" s="131"/>
-      <c r="I12" s="130"/>
-      <c r="J12" s="131"/>
-      <c r="K12" s="136"/>
+      <c r="G12" s="141"/>
+      <c r="H12" s="122"/>
+      <c r="I12" s="121"/>
+      <c r="J12" s="122"/>
+      <c r="K12" s="127"/>
       <c r="M12" s="3" t="s">
         <v>71</v>
       </c>
@@ -3391,24 +3438,24 @@
       <c r="AB12" s="25"/>
     </row>
     <row r="13" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="144"/>
-      <c r="C13" s="145"/>
-      <c r="D13" s="146"/>
-      <c r="E13" s="145"/>
-      <c r="F13" s="147"/>
-      <c r="G13" s="148" t="s">
+      <c r="B13" s="135"/>
+      <c r="C13" s="136"/>
+      <c r="D13" s="137"/>
+      <c r="E13" s="136"/>
+      <c r="F13" s="138"/>
+      <c r="G13" s="139" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="146" t="s">
+      <c r="H13" s="137" t="s">
         <v>80</v>
       </c>
-      <c r="I13" s="145" t="s">
+      <c r="I13" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="146" t="s">
+      <c r="J13" s="137" t="s">
         <v>15</v>
       </c>
-      <c r="K13" s="149" t="s">
+      <c r="K13" s="140" t="s">
         <v>18</v>
       </c>
       <c r="M13" s="20" t="s">
@@ -3426,8 +3473,8 @@
       <c r="T13" s="25"/>
       <c r="U13" s="25"/>
       <c r="V13" s="25"/>
-      <c r="W13" s="120"/>
-      <c r="X13" s="117"/>
+      <c r="W13" s="111"/>
+      <c r="X13" s="108"/>
       <c r="Y13" s="25"/>
       <c r="Z13" s="25"/>
       <c r="AA13" s="25"/>
@@ -3585,8 +3632,8 @@
       <c r="T19" s="25"/>
       <c r="U19" s="25"/>
       <c r="V19" s="25"/>
-      <c r="W19" s="120"/>
-      <c r="X19" s="117"/>
+      <c r="W19" s="111"/>
+      <c r="X19" s="108"/>
       <c r="Y19" s="25"/>
       <c r="Z19" s="25"/>
       <c r="AA19" s="25"/>
@@ -3675,8 +3722,8 @@
       <c r="I23" s="43"/>
       <c r="J23" s="43"/>
       <c r="K23" s="43"/>
-      <c r="Q23" s="120"/>
-      <c r="R23" s="117"/>
+      <c r="Q23" s="111"/>
+      <c r="R23" s="108"/>
       <c r="S23" s="25"/>
       <c r="T23" s="25"/>
       <c r="U23" s="25"/>
@@ -3777,8 +3824,8 @@
       <c r="T27" s="25"/>
       <c r="U27" s="25"/>
       <c r="V27" s="25"/>
-      <c r="W27" s="120"/>
-      <c r="X27" s="117"/>
+      <c r="W27" s="111"/>
+      <c r="X27" s="108"/>
       <c r="Y27" s="25"/>
       <c r="Z27" s="25"/>
       <c r="AA27" s="25"/>
@@ -3825,8 +3872,8 @@
       <c r="K30" s="25"/>
       <c r="L30" s="25"/>
       <c r="M30" s="25"/>
-      <c r="Q30" s="120"/>
-      <c r="R30" s="117"/>
+      <c r="Q30" s="111"/>
+      <c r="R30" s="108"/>
       <c r="S30" s="25"/>
       <c r="T30" s="25"/>
       <c r="U30" s="25"/>
@@ -4288,7 +4335,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O41"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4330,48 +4379,48 @@
       <c r="N3" s="42"/>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="70" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="151" t="s">
+      <c r="C4" s="142" t="s">
         <v>188</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
-      <c r="I4" s="81"/>
-      <c r="J4" s="81"/>
-      <c r="K4" s="81"/>
-      <c r="L4" s="81"/>
-      <c r="M4" s="81"/>
-      <c r="N4" s="82"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="73"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="104" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="152" t="s">
+      <c r="C5" s="143" t="s">
         <v>76</v>
       </c>
-      <c r="D5" s="114"/>
-      <c r="E5" s="114"/>
-      <c r="F5" s="114"/>
-      <c r="G5" s="114"/>
-      <c r="H5" s="114"/>
-      <c r="I5" s="114"/>
-      <c r="J5" s="114"/>
-      <c r="K5" s="114"/>
-      <c r="L5" s="114"/>
-      <c r="M5" s="114"/>
-      <c r="N5" s="115"/>
+      <c r="D5" s="105"/>
+      <c r="E5" s="105"/>
+      <c r="F5" s="105"/>
+      <c r="G5" s="105"/>
+      <c r="H5" s="105"/>
+      <c r="I5" s="105"/>
+      <c r="J5" s="105"/>
+      <c r="K5" s="105"/>
+      <c r="L5" s="105"/>
+      <c r="M5" s="105"/>
+      <c r="N5" s="106"/>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="153" t="s">
+      <c r="C6" s="144" t="s">
         <v>189</v>
       </c>
       <c r="D6" s="25"/>
@@ -4388,29 +4437,29 @@
       <c r="O6" s="25"/>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="116" t="s">
+      <c r="B7" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="C7" s="143" t="s">
         <v>190</v>
       </c>
-      <c r="D7" s="94"/>
-      <c r="E7" s="94"/>
-      <c r="F7" s="94"/>
-      <c r="G7" s="94"/>
-      <c r="H7" s="94"/>
-      <c r="I7" s="94"/>
-      <c r="J7" s="94"/>
-      <c r="K7" s="94"/>
-      <c r="L7" s="94"/>
-      <c r="M7" s="94"/>
-      <c r="N7" s="102"/>
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="85"/>
+      <c r="K7" s="85"/>
+      <c r="L7" s="85"/>
+      <c r="M7" s="85"/>
+      <c r="N7" s="93"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="153" t="s">
+      <c r="C8" s="144" t="s">
         <v>191</v>
       </c>
       <c r="D8" s="25"/>
@@ -4426,29 +4475,29 @@
       <c r="N8" s="45"/>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B9" s="116" t="s">
+      <c r="B9" s="107" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="152" t="s">
+      <c r="C9" s="143" t="s">
         <v>75</v>
       </c>
-      <c r="D9" s="94"/>
-      <c r="E9" s="94"/>
-      <c r="F9" s="94"/>
-      <c r="G9" s="94"/>
-      <c r="H9" s="94"/>
-      <c r="I9" s="94"/>
-      <c r="J9" s="94"/>
-      <c r="K9" s="94"/>
-      <c r="L9" s="94"/>
-      <c r="M9" s="94"/>
-      <c r="N9" s="102"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="93"/>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="153" t="s">
+      <c r="C10" s="144" t="s">
         <v>78</v>
       </c>
       <c r="D10" s="25"/>
@@ -4464,29 +4513,29 @@
       <c r="N10" s="45"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="107" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="152" t="s">
+      <c r="C11" s="143" t="s">
         <v>77</v>
       </c>
-      <c r="D11" s="94"/>
-      <c r="E11" s="94"/>
-      <c r="F11" s="94"/>
-      <c r="G11" s="94"/>
-      <c r="H11" s="94"/>
-      <c r="I11" s="94"/>
-      <c r="J11" s="94"/>
-      <c r="K11" s="94"/>
-      <c r="L11" s="94"/>
-      <c r="M11" s="94"/>
-      <c r="N11" s="102"/>
+      <c r="D11" s="85"/>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="85"/>
+      <c r="H11" s="85"/>
+      <c r="I11" s="85"/>
+      <c r="J11" s="85"/>
+      <c r="K11" s="85"/>
+      <c r="L11" s="85"/>
+      <c r="M11" s="85"/>
+      <c r="N11" s="93"/>
     </row>
     <row r="12" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="80" t="s">
+      <c r="B12" s="71" t="s">
         <v>80</v>
       </c>
-      <c r="C12" s="154" t="s">
+      <c r="C12" s="145" t="s">
         <v>79</v>
       </c>
       <c r="D12" s="47"/>
@@ -4880,7 +4929,7 @@
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B40" s="25"/>
-      <c r="H40" s="78"/>
+      <c r="H40" s="69"/>
     </row>
     <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B41" s="25"/>
@@ -4895,7 +4944,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:M33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -4939,42 +4990,42 @@
       <c r="M3" s="42"/>
     </row>
     <row r="4" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B4" s="121" t="s">
+      <c r="B4" s="112" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="103" t="s">
+      <c r="C4" s="94" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="104"/>
-      <c r="E4" s="104"/>
-      <c r="F4" s="104"/>
-      <c r="G4" s="105"/>
-      <c r="H4" s="97" t="s">
+      <c r="D4" s="95"/>
+      <c r="E4" s="95"/>
+      <c r="F4" s="95"/>
+      <c r="G4" s="96"/>
+      <c r="H4" s="88" t="s">
         <v>160</v>
       </c>
-      <c r="I4" s="98" t="s">
+      <c r="I4" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="J4" s="99"/>
-      <c r="K4" s="99"/>
-      <c r="L4" s="99"/>
-      <c r="M4" s="100"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="90"/>
+      <c r="L4" s="90"/>
+      <c r="M4" s="91"/>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="C5" s="83" t="s">
+      <c r="C5" s="74" t="s">
         <v>82</v>
       </c>
       <c r="D5" s="25"/>
       <c r="E5" s="25"/>
       <c r="F5" s="25"/>
-      <c r="G5" s="84"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="I5" s="85" t="s">
+      <c r="I5" s="76" t="s">
         <v>110</v>
       </c>
       <c r="J5" s="25"/>
@@ -4983,42 +5034,42 @@
       <c r="M5" s="45"/>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="97" t="s">
         <v>135</v>
       </c>
-      <c r="C6" s="107" t="s">
+      <c r="C6" s="98" t="s">
         <v>83</v>
       </c>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
-      <c r="F6" s="108"/>
-      <c r="G6" s="109"/>
-      <c r="H6" s="101" t="s">
+      <c r="D6" s="99"/>
+      <c r="E6" s="99"/>
+      <c r="F6" s="99"/>
+      <c r="G6" s="100"/>
+      <c r="H6" s="92" t="s">
         <v>162</v>
       </c>
-      <c r="I6" s="96" t="s">
+      <c r="I6" s="87" t="s">
         <v>104</v>
       </c>
-      <c r="J6" s="94"/>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="102"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="93"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="C7" s="83" t="s">
+      <c r="C7" s="74" t="s">
         <v>84</v>
       </c>
       <c r="D7" s="25"/>
       <c r="E7" s="25"/>
       <c r="F7" s="25"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="120" t="s">
+      <c r="G7" s="75"/>
+      <c r="H7" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="86" t="s">
+      <c r="I7" s="77" t="s">
         <v>105</v>
       </c>
       <c r="J7" s="25"/>
@@ -5027,42 +5078,42 @@
       <c r="M7" s="45"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="97" t="s">
         <v>137</v>
       </c>
-      <c r="C8" s="107" t="s">
+      <c r="C8" s="98" t="s">
         <v>86</v>
       </c>
-      <c r="D8" s="108"/>
-      <c r="E8" s="108"/>
-      <c r="F8" s="108"/>
-      <c r="G8" s="109"/>
-      <c r="H8" s="110" t="s">
+      <c r="D8" s="99"/>
+      <c r="E8" s="99"/>
+      <c r="F8" s="99"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="101" t="s">
         <v>163</v>
       </c>
-      <c r="I8" s="107" t="s">
+      <c r="I8" s="98" t="s">
         <v>111</v>
       </c>
-      <c r="J8" s="108"/>
-      <c r="K8" s="108"/>
-      <c r="L8" s="108"/>
-      <c r="M8" s="111"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="102"/>
     </row>
     <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="C9" s="85" t="s">
+      <c r="C9" s="76" t="s">
         <v>104</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
-      <c r="G9" s="84"/>
+      <c r="G9" s="75"/>
       <c r="H9" s="43" t="s">
         <v>164</v>
       </c>
-      <c r="I9" s="85" t="s">
+      <c r="I9" s="76" t="s">
         <v>112</v>
       </c>
       <c r="J9" s="25"/>
@@ -5071,42 +5122,42 @@
       <c r="M9" s="45"/>
     </row>
     <row r="10" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B10" s="122" t="s">
+      <c r="B10" s="113" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="93" t="s">
+      <c r="C10" s="84" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="94"/>
-      <c r="E10" s="94"/>
-      <c r="F10" s="94"/>
-      <c r="G10" s="95"/>
-      <c r="H10" s="110" t="s">
+      <c r="D10" s="85"/>
+      <c r="E10" s="85"/>
+      <c r="F10" s="85"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="101" t="s">
         <v>165</v>
       </c>
-      <c r="I10" s="107" t="s">
+      <c r="I10" s="98" t="s">
         <v>113</v>
       </c>
-      <c r="J10" s="108"/>
-      <c r="K10" s="108"/>
-      <c r="L10" s="108"/>
-      <c r="M10" s="111"/>
+      <c r="J10" s="99"/>
+      <c r="K10" s="99"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="102"/>
     </row>
     <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="C11" s="85" t="s">
+      <c r="C11" s="76" t="s">
         <v>132</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
-      <c r="G11" s="84"/>
+      <c r="G11" s="75"/>
       <c r="H11" s="43" t="s">
         <v>166</v>
       </c>
-      <c r="I11" s="85" t="s">
+      <c r="I11" s="76" t="s">
         <v>114</v>
       </c>
       <c r="J11" s="25"/>
@@ -5115,42 +5166,42 @@
       <c r="M11" s="45"/>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="92" t="s">
+      <c r="B12" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="C12" s="96" t="s">
+      <c r="C12" s="87" t="s">
         <v>133</v>
       </c>
-      <c r="D12" s="94"/>
-      <c r="E12" s="94"/>
-      <c r="F12" s="94"/>
-      <c r="G12" s="95"/>
-      <c r="H12" s="110" t="s">
+      <c r="D12" s="85"/>
+      <c r="E12" s="85"/>
+      <c r="F12" s="85"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="101" t="s">
         <v>167</v>
       </c>
-      <c r="I12" s="107" t="s">
+      <c r="I12" s="98" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="108"/>
-      <c r="K12" s="108"/>
-      <c r="L12" s="108"/>
-      <c r="M12" s="111"/>
+      <c r="J12" s="99"/>
+      <c r="K12" s="99"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="102"/>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="C13" s="85" t="s">
+      <c r="C13" s="76" t="s">
         <v>90</v>
       </c>
       <c r="D13" s="25"/>
       <c r="E13" s="25"/>
       <c r="F13" s="25"/>
-      <c r="G13" s="84"/>
+      <c r="G13" s="75"/>
       <c r="H13" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="76" t="s">
         <v>116</v>
       </c>
       <c r="J13" s="25"/>
@@ -5159,42 +5210,42 @@
       <c r="M13" s="45"/>
     </row>
     <row r="14" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B14" s="92" t="s">
+      <c r="B14" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="C14" s="96" t="s">
+      <c r="C14" s="87" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="94"/>
-      <c r="E14" s="94"/>
-      <c r="F14" s="94"/>
-      <c r="G14" s="95"/>
-      <c r="H14" s="118" t="s">
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="109" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="93" t="s">
+      <c r="I14" s="84" t="s">
         <v>117</v>
       </c>
-      <c r="J14" s="94"/>
-      <c r="K14" s="94"/>
-      <c r="L14" s="94"/>
-      <c r="M14" s="102"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="93"/>
     </row>
     <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C15" s="85" t="s">
+      <c r="C15" s="76" t="s">
         <v>92</v>
       </c>
       <c r="D15" s="25"/>
       <c r="E15" s="25"/>
       <c r="F15" s="25"/>
-      <c r="G15" s="84"/>
+      <c r="G15" s="75"/>
       <c r="H15" s="43" t="s">
         <v>169</v>
       </c>
-      <c r="I15" s="85" t="s">
+      <c r="I15" s="76" t="s">
         <v>118</v>
       </c>
       <c r="J15" s="25"/>
@@ -5203,42 +5254,42 @@
       <c r="M15" s="45"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B16" s="92" t="s">
+      <c r="B16" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="C16" s="96" t="s">
+      <c r="C16" s="87" t="s">
         <v>93</v>
       </c>
-      <c r="D16" s="94"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="94"/>
-      <c r="G16" s="95"/>
-      <c r="H16" s="101" t="s">
+      <c r="D16" s="85"/>
+      <c r="E16" s="85"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="92" t="s">
         <v>170</v>
       </c>
-      <c r="I16" s="96" t="s">
+      <c r="I16" s="87" t="s">
         <v>119</v>
       </c>
-      <c r="J16" s="94"/>
-      <c r="K16" s="94"/>
-      <c r="L16" s="94"/>
-      <c r="M16" s="102"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="85"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="93"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="76" t="s">
         <v>94</v>
       </c>
       <c r="D17" s="25"/>
       <c r="E17" s="25"/>
       <c r="F17" s="25"/>
-      <c r="G17" s="84"/>
+      <c r="G17" s="75"/>
       <c r="H17" s="43" t="s">
         <v>171</v>
       </c>
-      <c r="I17" s="85" t="s">
+      <c r="I17" s="76" t="s">
         <v>120</v>
       </c>
       <c r="J17" s="25"/>
@@ -5247,42 +5298,42 @@
       <c r="M17" s="45"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="C18" s="96" t="s">
+      <c r="C18" s="87" t="s">
         <v>95</v>
       </c>
-      <c r="D18" s="94"/>
-      <c r="E18" s="94"/>
-      <c r="F18" s="94"/>
-      <c r="G18" s="95"/>
-      <c r="H18" s="101" t="s">
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I18" s="96" t="s">
+      <c r="I18" s="87" t="s">
         <v>121</v>
       </c>
-      <c r="J18" s="94"/>
-      <c r="K18" s="94"/>
-      <c r="L18" s="94"/>
-      <c r="M18" s="102"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
+      <c r="L18" s="85"/>
+      <c r="M18" s="93"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="44" t="s">
         <v>147</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="76" t="s">
         <v>96</v>
       </c>
       <c r="D19" s="25"/>
       <c r="E19" s="25"/>
       <c r="F19" s="25"/>
-      <c r="G19" s="84"/>
+      <c r="G19" s="75"/>
       <c r="H19" s="43" t="s">
         <v>173</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="76" t="s">
         <v>104</v>
       </c>
       <c r="J19" s="25"/>
@@ -5291,42 +5342,42 @@
       <c r="M19" s="45"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="92" t="s">
+      <c r="B20" s="83" t="s">
         <v>148</v>
       </c>
-      <c r="C20" s="96" t="s">
+      <c r="C20" s="87" t="s">
         <v>97</v>
       </c>
-      <c r="D20" s="94"/>
-      <c r="E20" s="94"/>
-      <c r="F20" s="94"/>
-      <c r="G20" s="95"/>
-      <c r="H20" s="119" t="s">
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="110" t="s">
         <v>27</v>
       </c>
-      <c r="I20" s="112" t="s">
+      <c r="I20" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="J20" s="108"/>
-      <c r="K20" s="108"/>
-      <c r="L20" s="108"/>
-      <c r="M20" s="111"/>
+      <c r="J20" s="99"/>
+      <c r="K20" s="99"/>
+      <c r="L20" s="99"/>
+      <c r="M20" s="102"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="C21" s="85" t="s">
+      <c r="C21" s="76" t="s">
         <v>98</v>
       </c>
       <c r="D21" s="25"/>
       <c r="E21" s="25"/>
       <c r="F21" s="25"/>
-      <c r="G21" s="84"/>
+      <c r="G21" s="75"/>
       <c r="H21" s="43" t="s">
         <v>174</v>
       </c>
-      <c r="I21" s="85" t="s">
+      <c r="I21" s="76" t="s">
         <v>111</v>
       </c>
       <c r="J21" s="25"/>
@@ -5335,42 +5386,42 @@
       <c r="M21" s="45"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="92" t="s">
+      <c r="B22" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="C22" s="96" t="s">
+      <c r="C22" s="87" t="s">
         <v>99</v>
       </c>
-      <c r="D22" s="94"/>
-      <c r="E22" s="94"/>
-      <c r="F22" s="94"/>
-      <c r="G22" s="95"/>
-      <c r="H22" s="110" t="s">
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="86"/>
+      <c r="H22" s="101" t="s">
         <v>175</v>
       </c>
-      <c r="I22" s="107" t="s">
+      <c r="I22" s="98" t="s">
         <v>125</v>
       </c>
-      <c r="J22" s="108"/>
-      <c r="K22" s="108"/>
-      <c r="L22" s="108"/>
-      <c r="M22" s="111"/>
+      <c r="J22" s="99"/>
+      <c r="K22" s="99"/>
+      <c r="L22" s="99"/>
+      <c r="M22" s="102"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="C23" s="85" t="s">
+      <c r="C23" s="76" t="s">
         <v>87</v>
       </c>
       <c r="D23" s="25"/>
       <c r="E23" s="25"/>
       <c r="F23" s="25"/>
-      <c r="G23" s="84"/>
+      <c r="G23" s="75"/>
       <c r="H23" s="43" t="s">
         <v>176</v>
       </c>
-      <c r="I23" s="85" t="s">
+      <c r="I23" s="76" t="s">
         <v>123</v>
       </c>
       <c r="J23" s="25"/>
@@ -5379,42 +5430,42 @@
       <c r="M23" s="45"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B24" s="123" t="s">
+      <c r="B24" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="112" t="s">
+      <c r="C24" s="103" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="108"/>
-      <c r="E24" s="108"/>
-      <c r="F24" s="108"/>
-      <c r="G24" s="109"/>
-      <c r="H24" s="110" t="s">
+      <c r="D24" s="99"/>
+      <c r="E24" s="99"/>
+      <c r="F24" s="99"/>
+      <c r="G24" s="100"/>
+      <c r="H24" s="101" t="s">
         <v>177</v>
       </c>
-      <c r="I24" s="107" t="s">
+      <c r="I24" s="98" t="s">
         <v>124</v>
       </c>
-      <c r="J24" s="108"/>
-      <c r="K24" s="108"/>
-      <c r="L24" s="108"/>
-      <c r="M24" s="111"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="102"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="C25" s="85" t="s">
+      <c r="C25" s="76" t="s">
         <v>132</v>
       </c>
       <c r="D25" s="25"/>
       <c r="E25" s="25"/>
       <c r="F25" s="25"/>
-      <c r="G25" s="84"/>
+      <c r="G25" s="75"/>
       <c r="H25" s="43" t="s">
         <v>178</v>
       </c>
-      <c r="I25" s="85" t="s">
+      <c r="I25" s="76" t="s">
         <v>126</v>
       </c>
       <c r="J25" s="25"/>
@@ -5424,43 +5475,43 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="25"/>
-      <c r="B26" s="106" t="s">
+      <c r="B26" s="97" t="s">
         <v>153</v>
       </c>
-      <c r="C26" s="107" t="s">
+      <c r="C26" s="98" t="s">
         <v>100</v>
       </c>
-      <c r="D26" s="108"/>
-      <c r="E26" s="108"/>
-      <c r="F26" s="108"/>
-      <c r="G26" s="109"/>
-      <c r="H26" s="110" t="s">
+      <c r="D26" s="99"/>
+      <c r="E26" s="99"/>
+      <c r="F26" s="99"/>
+      <c r="G26" s="100"/>
+      <c r="H26" s="101" t="s">
         <v>179</v>
       </c>
-      <c r="I26" s="107" t="s">
+      <c r="I26" s="98" t="s">
         <v>127</v>
       </c>
-      <c r="J26" s="108"/>
-      <c r="K26" s="108"/>
-      <c r="L26" s="108"/>
-      <c r="M26" s="111"/>
+      <c r="J26" s="99"/>
+      <c r="K26" s="99"/>
+      <c r="L26" s="99"/>
+      <c r="M26" s="102"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="25"/>
       <c r="B27" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C27" s="76" t="s">
         <v>89</v>
       </c>
       <c r="D27" s="25"/>
       <c r="E27" s="25"/>
       <c r="F27" s="25"/>
-      <c r="G27" s="84"/>
+      <c r="G27" s="75"/>
       <c r="H27" s="43" t="s">
         <v>180</v>
       </c>
-      <c r="I27" s="85" t="s">
+      <c r="I27" s="76" t="s">
         <v>87</v>
       </c>
       <c r="J27" s="25"/>
@@ -5470,43 +5521,43 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="25"/>
-      <c r="B28" s="106" t="s">
+      <c r="B28" s="97" t="s">
         <v>155</v>
       </c>
-      <c r="C28" s="107" t="s">
+      <c r="C28" s="98" t="s">
         <v>102</v>
       </c>
-      <c r="D28" s="108"/>
-      <c r="E28" s="108"/>
-      <c r="F28" s="108"/>
-      <c r="G28" s="109"/>
-      <c r="H28" s="118" t="s">
+      <c r="D28" s="99"/>
+      <c r="E28" s="99"/>
+      <c r="F28" s="99"/>
+      <c r="G28" s="100"/>
+      <c r="H28" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="I28" s="93" t="s">
+      <c r="I28" s="84" t="s">
         <v>128</v>
       </c>
-      <c r="J28" s="94"/>
-      <c r="K28" s="94"/>
-      <c r="L28" s="94"/>
-      <c r="M28" s="102"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="93"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="25"/>
       <c r="B29" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="C29" s="85" t="s">
+      <c r="C29" s="76" t="s">
         <v>101</v>
       </c>
       <c r="D29" s="25"/>
       <c r="E29" s="25"/>
       <c r="F29" s="25"/>
-      <c r="G29" s="84"/>
+      <c r="G29" s="75"/>
       <c r="H29" s="43" t="s">
         <v>181</v>
       </c>
-      <c r="I29" s="85" t="s">
+      <c r="I29" s="76" t="s">
         <v>129</v>
       </c>
       <c r="J29" s="25"/>
@@ -5516,42 +5567,42 @@
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="25"/>
-      <c r="B30" s="106" t="s">
+      <c r="B30" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="107" t="s">
+      <c r="C30" s="98" t="s">
         <v>103</v>
       </c>
-      <c r="D30" s="108"/>
-      <c r="E30" s="108"/>
-      <c r="F30" s="108"/>
-      <c r="G30" s="109"/>
-      <c r="H30" s="101" t="s">
+      <c r="D30" s="99"/>
+      <c r="E30" s="99"/>
+      <c r="F30" s="99"/>
+      <c r="G30" s="100"/>
+      <c r="H30" s="92" t="s">
         <v>182</v>
       </c>
-      <c r="I30" s="96" t="s">
+      <c r="I30" s="87" t="s">
         <v>131</v>
       </c>
-      <c r="J30" s="94"/>
-      <c r="K30" s="94"/>
-      <c r="L30" s="94"/>
-      <c r="M30" s="102"/>
+      <c r="J30" s="85"/>
+      <c r="K30" s="85"/>
+      <c r="L30" s="85"/>
+      <c r="M30" s="93"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B31" s="124" t="s">
+      <c r="B31" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="86" t="s">
+      <c r="C31" s="77" t="s">
         <v>106</v>
       </c>
       <c r="D31" s="25"/>
       <c r="E31" s="25"/>
       <c r="F31" s="25"/>
-      <c r="G31" s="84"/>
+      <c r="G31" s="75"/>
       <c r="H31" s="43" t="s">
         <v>183</v>
       </c>
-      <c r="I31" s="85" t="s">
+      <c r="I31" s="76" t="s">
         <v>130</v>
       </c>
       <c r="J31" s="25"/>
@@ -5560,44 +5611,44 @@
       <c r="M31" s="45"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B32" s="92" t="s">
+      <c r="B32" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="C32" s="96" t="s">
+      <c r="C32" s="87" t="s">
         <v>107</v>
       </c>
-      <c r="D32" s="94"/>
-      <c r="E32" s="94"/>
-      <c r="F32" s="94"/>
-      <c r="G32" s="95"/>
-      <c r="H32" s="101" t="s">
+      <c r="D32" s="85"/>
+      <c r="E32" s="85"/>
+      <c r="F32" s="85"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="92" t="s">
         <v>184</v>
       </c>
-      <c r="I32" s="96" t="s">
+      <c r="I32" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="J32" s="94"/>
-      <c r="K32" s="94"/>
-      <c r="L32" s="94"/>
-      <c r="M32" s="102"/>
+      <c r="J32" s="85"/>
+      <c r="K32" s="85"/>
+      <c r="L32" s="85"/>
+      <c r="M32" s="93"/>
     </row>
     <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="58" t="s">
         <v>159</v>
       </c>
-      <c r="C33" s="91" t="s">
+      <c r="C33" s="82" t="s">
         <v>108</v>
       </c>
-      <c r="D33" s="87"/>
-      <c r="E33" s="87"/>
-      <c r="F33" s="87"/>
-      <c r="G33" s="88"/>
+      <c r="D33" s="78"/>
+      <c r="E33" s="78"/>
+      <c r="F33" s="78"/>
+      <c r="G33" s="79"/>
       <c r="H33" s="48"/>
-      <c r="I33" s="89"/>
-      <c r="J33" s="87"/>
-      <c r="K33" s="87"/>
-      <c r="L33" s="87"/>
-      <c r="M33" s="90"/>
+      <c r="I33" s="80"/>
+      <c r="J33" s="78"/>
+      <c r="K33" s="78"/>
+      <c r="L33" s="78"/>
+      <c r="M33" s="81"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5610,13 +5661,13 @@
   <dimension ref="B1:Q35"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="B2" sqref="B2:M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="35.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5637,8 +5688,8 @@
       <c r="L2" s="28"/>
       <c r="M2" s="30"/>
     </row>
-    <row r="3" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B3" s="71" t="s">
+    <row r="3" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="65" t="s">
         <v>40</v>
       </c>
       <c r="C3" s="50" t="s">
@@ -5671,44 +5722,48 @@
       <c r="L3" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="M3" s="72" t="s">
+      <c r="M3" s="66" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B4" s="64" t="s">
+      <c r="B4" s="154" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="65" t="s">
+      <c r="C4" s="162" t="s">
         <v>64</v>
       </c>
-      <c r="D4" s="66">
+      <c r="D4" s="129">
         <v>8</v>
       </c>
-      <c r="E4" s="59">
-        <f t="shared" ref="E4:E17" si="0">D4</f>
+      <c r="E4" s="157">
+        <f t="shared" ref="E4:E19" si="0">D4</f>
         <v>8</v>
       </c>
-      <c r="F4" s="76">
-        <v>0</v>
-      </c>
-      <c r="G4" s="76">
-        <v>0</v>
-      </c>
-      <c r="H4" s="76">
-        <v>0</v>
-      </c>
-      <c r="I4" s="76">
-        <v>0</v>
-      </c>
-      <c r="J4" s="76">
-        <v>0</v>
-      </c>
-      <c r="K4" s="76">
-        <v>0</v>
-      </c>
-      <c r="L4" s="76"/>
-      <c r="M4" s="77"/>
+      <c r="F4" s="155">
+        <v>0</v>
+      </c>
+      <c r="G4" s="155">
+        <v>0</v>
+      </c>
+      <c r="H4" s="155">
+        <v>0</v>
+      </c>
+      <c r="I4" s="155">
+        <v>0</v>
+      </c>
+      <c r="J4" s="155">
+        <v>0</v>
+      </c>
+      <c r="K4" s="155">
+        <v>0</v>
+      </c>
+      <c r="L4" s="155">
+        <v>0</v>
+      </c>
+      <c r="M4" s="156">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B5" s="31" t="s">
@@ -5717,33 +5772,37 @@
       <c r="C5" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="D5" s="67">
+      <c r="D5" s="160">
         <v>11</v>
       </c>
-      <c r="E5" s="59">
+      <c r="E5" s="158">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="F5" s="76">
-        <v>0</v>
-      </c>
-      <c r="G5" s="76">
-        <v>0</v>
-      </c>
-      <c r="H5" s="76">
-        <v>0</v>
-      </c>
-      <c r="I5" s="76">
-        <v>0</v>
-      </c>
-      <c r="J5" s="76">
-        <v>0</v>
-      </c>
-      <c r="K5" s="76">
-        <v>0</v>
-      </c>
-      <c r="L5" s="76"/>
-      <c r="M5" s="77"/>
+      <c r="F5" s="67">
+        <v>0</v>
+      </c>
+      <c r="G5" s="67">
+        <v>0</v>
+      </c>
+      <c r="H5" s="67">
+        <v>0</v>
+      </c>
+      <c r="I5" s="67">
+        <v>0</v>
+      </c>
+      <c r="J5" s="67">
+        <v>0</v>
+      </c>
+      <c r="K5" s="67">
+        <v>0</v>
+      </c>
+      <c r="L5" s="67">
+        <v>0</v>
+      </c>
+      <c r="M5" s="68">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="10" t="s">
@@ -5752,33 +5811,37 @@
       <c r="C6" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D6" s="68">
+      <c r="D6" s="117">
         <v>12</v>
       </c>
-      <c r="E6" s="59">
+      <c r="E6" s="158">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="F6" s="59">
         <v>12</v>
       </c>
-      <c r="G6" s="76">
-        <v>0</v>
-      </c>
-      <c r="H6" s="76">
-        <v>0</v>
-      </c>
-      <c r="I6" s="76">
-        <v>0</v>
-      </c>
-      <c r="J6" s="76">
-        <v>0</v>
-      </c>
-      <c r="K6" s="76">
-        <v>0</v>
-      </c>
-      <c r="L6" s="76"/>
-      <c r="M6" s="77"/>
+      <c r="G6" s="67">
+        <v>0</v>
+      </c>
+      <c r="H6" s="67">
+        <v>0</v>
+      </c>
+      <c r="I6" s="67">
+        <v>0</v>
+      </c>
+      <c r="J6" s="67">
+        <v>0</v>
+      </c>
+      <c r="K6" s="67">
+        <v>0</v>
+      </c>
+      <c r="L6" s="67">
+        <v>0</v>
+      </c>
+      <c r="M6" s="68">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B7" s="31" t="s">
@@ -5787,10 +5850,10 @@
       <c r="C7" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="D7" s="67">
+      <c r="D7" s="160">
         <v>12</v>
       </c>
-      <c r="E7" s="59">
+      <c r="E7" s="158">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -5803,17 +5866,21 @@
       <c r="H7" s="59">
         <v>13</v>
       </c>
-      <c r="I7" s="76">
-        <v>0</v>
-      </c>
-      <c r="J7" s="76">
-        <v>0</v>
-      </c>
-      <c r="K7" s="76">
-        <v>0</v>
-      </c>
-      <c r="L7" s="76"/>
-      <c r="M7" s="77"/>
+      <c r="I7" s="67">
+        <v>0</v>
+      </c>
+      <c r="J7" s="67">
+        <v>0</v>
+      </c>
+      <c r="K7" s="67">
+        <v>0</v>
+      </c>
+      <c r="L7" s="67">
+        <v>0</v>
+      </c>
+      <c r="M7" s="68">
+        <v>0</v>
+      </c>
       <c r="O7" s="12"/>
       <c r="P7" s="14" t="s">
         <v>7</v>
@@ -5827,10 +5894,10 @@
       <c r="C8" s="62" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="68">
+      <c r="D8" s="117">
         <v>12</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="158">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -5843,17 +5910,21 @@
       <c r="H8" s="59">
         <v>13</v>
       </c>
-      <c r="I8" s="76">
-        <v>0</v>
-      </c>
-      <c r="J8" s="76">
-        <v>0</v>
-      </c>
-      <c r="K8" s="76">
-        <v>0</v>
-      </c>
-      <c r="L8" s="76"/>
-      <c r="M8" s="77"/>
+      <c r="I8" s="67">
+        <v>0</v>
+      </c>
+      <c r="J8" s="67">
+        <v>0</v>
+      </c>
+      <c r="K8" s="67">
+        <v>0</v>
+      </c>
+      <c r="L8" s="67">
+        <v>0</v>
+      </c>
+      <c r="M8" s="68">
+        <v>0</v>
+      </c>
       <c r="O8" s="36" t="s">
         <v>9</v>
       </c>
@@ -5869,33 +5940,37 @@
       <c r="C9" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="67">
+      <c r="D9" s="160">
         <v>12</v>
       </c>
-      <c r="E9" s="59">
+      <c r="E9" s="158">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="F9" s="76">
-        <v>0</v>
-      </c>
-      <c r="G9" s="76">
-        <v>0</v>
-      </c>
-      <c r="H9" s="76">
-        <v>0</v>
-      </c>
-      <c r="I9" s="76">
-        <v>0</v>
-      </c>
-      <c r="J9" s="76">
-        <v>0</v>
-      </c>
-      <c r="K9" s="76">
-        <v>0</v>
-      </c>
-      <c r="L9" s="76"/>
-      <c r="M9" s="77"/>
+      <c r="F9" s="67">
+        <v>0</v>
+      </c>
+      <c r="G9" s="67">
+        <v>0</v>
+      </c>
+      <c r="H9" s="67">
+        <v>0</v>
+      </c>
+      <c r="I9" s="67">
+        <v>0</v>
+      </c>
+      <c r="J9" s="67">
+        <v>0</v>
+      </c>
+      <c r="K9" s="67">
+        <v>0</v>
+      </c>
+      <c r="L9" s="67">
+        <v>0</v>
+      </c>
+      <c r="M9" s="68">
+        <v>0</v>
+      </c>
       <c r="O9" s="3" t="s">
         <v>69</v>
       </c>
@@ -5913,33 +5988,37 @@
       <c r="C10" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="68">
+      <c r="D10" s="117">
         <v>4</v>
       </c>
-      <c r="E10" s="59">
+      <c r="E10" s="158">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F10" s="76">
-        <v>0</v>
-      </c>
-      <c r="G10" s="76">
-        <v>0</v>
-      </c>
-      <c r="H10" s="76">
-        <v>0</v>
-      </c>
-      <c r="I10" s="76">
-        <v>0</v>
-      </c>
-      <c r="J10" s="76">
-        <v>0</v>
-      </c>
-      <c r="K10" s="76">
-        <v>0</v>
-      </c>
-      <c r="L10" s="76"/>
-      <c r="M10" s="77"/>
+      <c r="F10" s="67">
+        <v>0</v>
+      </c>
+      <c r="G10" s="67">
+        <v>0</v>
+      </c>
+      <c r="H10" s="67">
+        <v>0</v>
+      </c>
+      <c r="I10" s="67">
+        <v>0</v>
+      </c>
+      <c r="J10" s="67">
+        <v>0</v>
+      </c>
+      <c r="K10" s="67">
+        <v>0</v>
+      </c>
+      <c r="L10" s="67">
+        <v>0</v>
+      </c>
+      <c r="M10" s="68">
+        <v>0</v>
+      </c>
       <c r="O10" s="20" t="s">
         <v>70</v>
       </c>
@@ -5957,10 +6036,10 @@
       <c r="C11" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D11" s="67">
+      <c r="D11" s="160">
         <v>13</v>
       </c>
-      <c r="E11" s="59">
+      <c r="E11" s="158">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -5973,17 +6052,21 @@
       <c r="H11" s="59">
         <v>14</v>
       </c>
-      <c r="I11" s="76">
-        <v>0</v>
-      </c>
-      <c r="J11" s="76">
-        <v>0</v>
-      </c>
-      <c r="K11" s="76">
-        <v>0</v>
-      </c>
-      <c r="L11" s="76"/>
-      <c r="M11" s="77"/>
+      <c r="I11" s="67">
+        <v>0</v>
+      </c>
+      <c r="J11" s="67">
+        <v>0</v>
+      </c>
+      <c r="K11" s="67">
+        <v>0</v>
+      </c>
+      <c r="L11" s="67">
+        <v>0</v>
+      </c>
+      <c r="M11" s="68">
+        <v>0</v>
+      </c>
       <c r="O11" s="3" t="s">
         <v>71</v>
       </c>
@@ -6001,10 +6084,10 @@
       <c r="C12" s="62" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="68">
+      <c r="D12" s="117">
         <v>12</v>
       </c>
-      <c r="E12" s="59">
+      <c r="E12" s="158">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
@@ -6023,11 +6106,15 @@
       <c r="J12" s="59">
         <v>10</v>
       </c>
-      <c r="K12" s="155">
-        <v>0</v>
-      </c>
-      <c r="L12" s="155"/>
-      <c r="M12" s="156"/>
+      <c r="K12" s="146">
+        <v>0</v>
+      </c>
+      <c r="L12" s="146">
+        <v>0</v>
+      </c>
+      <c r="M12" s="147">
+        <v>0</v>
+      </c>
       <c r="O12" s="20" t="s">
         <v>72</v>
       </c>
@@ -6045,10 +6132,10 @@
       <c r="C13" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="160">
         <v>13</v>
       </c>
-      <c r="E13" s="59">
+      <c r="E13" s="158">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
@@ -6070,8 +6157,12 @@
       <c r="K13" s="59">
         <v>13</v>
       </c>
-      <c r="L13" s="59"/>
-      <c r="M13" s="73"/>
+      <c r="L13" s="67">
+        <v>0</v>
+      </c>
+      <c r="M13" s="68">
+        <v>0</v>
+      </c>
       <c r="O13" s="3" t="s">
         <v>73</v>
       </c>
@@ -6089,10 +6180,10 @@
       <c r="C14" s="62" t="s">
         <v>65</v>
       </c>
-      <c r="D14" s="68">
+      <c r="D14" s="117">
         <v>15</v>
       </c>
-      <c r="E14" s="59">
+      <c r="E14" s="158">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -6114,8 +6205,12 @@
       <c r="K14" s="59">
         <v>15</v>
       </c>
-      <c r="L14" s="59"/>
-      <c r="M14" s="73"/>
+      <c r="L14" s="67">
+        <v>0</v>
+      </c>
+      <c r="M14" s="68">
+        <v>0</v>
+      </c>
       <c r="O14" s="22" t="s">
         <v>74</v>
       </c>
@@ -6133,10 +6228,10 @@
       <c r="C15" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D15" s="67">
+      <c r="D15" s="160">
         <v>15</v>
       </c>
-      <c r="E15" s="59">
+      <c r="E15" s="158">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
@@ -6158,8 +6253,12 @@
       <c r="K15" s="59">
         <v>15</v>
       </c>
-      <c r="L15" s="59"/>
-      <c r="M15" s="73"/>
+      <c r="L15" s="59">
+        <v>15</v>
+      </c>
+      <c r="M15" s="68">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
@@ -6168,33 +6267,37 @@
       <c r="C16" s="62" t="s">
         <v>187</v>
       </c>
-      <c r="D16" s="68">
+      <c r="D16" s="117">
         <v>11</v>
       </c>
-      <c r="E16" s="59">
+      <c r="E16" s="158">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="F16" s="59">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G16" s="59">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="H16" s="59">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="I16" s="59">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J16" s="59">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K16" s="59">
-        <v>13</v>
-      </c>
-      <c r="L16" s="59"/>
-      <c r="M16" s="73"/>
+        <v>11</v>
+      </c>
+      <c r="L16" s="59">
+        <v>11</v>
+      </c>
+      <c r="M16" s="68">
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" s="31" t="s">
@@ -6203,91 +6306,173 @@
       <c r="C17" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="67">
+      <c r="D17" s="160">
         <v>15</v>
       </c>
-      <c r="E17" s="59">
+      <c r="E17" s="158">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="F17" s="59">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="G17" s="59">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H17" s="59">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="I17" s="59">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J17" s="59">
-        <v>13</v>
-      </c>
-      <c r="K17" s="76">
-        <v>0</v>
-      </c>
-      <c r="L17" s="76"/>
-      <c r="M17" s="77"/>
-    </row>
-    <row r="18" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="46"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
-      <c r="I18" s="74"/>
-      <c r="J18" s="74"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="74"/>
-      <c r="M18" s="75"/>
-    </row>
-    <row r="19" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="9"/>
-      <c r="C19" s="70" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="67">
+        <v>0</v>
+      </c>
+      <c r="L17" s="67">
+        <v>0</v>
+      </c>
+      <c r="M17" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="148" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="149" t="s">
+        <v>194</v>
+      </c>
+      <c r="D18" s="161">
+        <v>18</v>
+      </c>
+      <c r="E18" s="158">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F18" s="150">
+        <v>18</v>
+      </c>
+      <c r="G18" s="150">
+        <v>18</v>
+      </c>
+      <c r="H18" s="150">
+        <v>18</v>
+      </c>
+      <c r="I18" s="150">
+        <v>18</v>
+      </c>
+      <c r="J18" s="150">
+        <v>18</v>
+      </c>
+      <c r="K18" s="150">
+        <v>18</v>
+      </c>
+      <c r="L18" s="150">
+        <v>18</v>
+      </c>
+      <c r="M18" s="164">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="63" t="s">
+        <v>195</v>
+      </c>
+      <c r="D19" s="160">
+        <v>17</v>
+      </c>
+      <c r="E19" s="158">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F19" s="153">
+        <v>17</v>
+      </c>
+      <c r="G19" s="153">
+        <v>17</v>
+      </c>
+      <c r="H19" s="153">
+        <v>17</v>
+      </c>
+      <c r="I19" s="153">
+        <v>17</v>
+      </c>
+      <c r="J19" s="153">
+        <v>17</v>
+      </c>
+      <c r="K19" s="153">
+        <v>17</v>
+      </c>
+      <c r="L19" s="153">
+        <v>17</v>
+      </c>
+      <c r="M19" s="68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="46"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="163"/>
+      <c r="E20" s="159"/>
+      <c r="F20" s="151"/>
+      <c r="G20" s="151"/>
+      <c r="H20" s="151"/>
+      <c r="I20" s="151"/>
+      <c r="J20" s="151"/>
+      <c r="K20" s="151"/>
+      <c r="L20" s="151"/>
+      <c r="M20" s="152"/>
+    </row>
+    <row r="21" spans="2:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="9"/>
+      <c r="C21" s="64" t="s">
         <v>52</v>
       </c>
-      <c r="D19" s="51">
-        <f t="shared" ref="D19:M19" si="1">D17+D16+D15+D14+D13+D12+D11+D10+D9+D8+D7+D6+D4+D5</f>
-        <v>165</v>
-      </c>
-      <c r="E19" s="51">
-        <f t="shared" si="1"/>
-        <v>165</v>
-      </c>
-      <c r="F19" s="51">
-        <f t="shared" si="1"/>
-        <v>131</v>
-      </c>
-      <c r="G19" s="51">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="H19" s="51">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-      <c r="I19" s="51">
-        <f t="shared" si="1"/>
-        <v>79</v>
-      </c>
-      <c r="J19" s="51">
-        <f t="shared" ref="J19" si="2">J17+J16+J15+J14+J13+J12+J11+J10+J9+J8+J7+J6+J4+J5</f>
-        <v>79</v>
-      </c>
-      <c r="K19" s="51">
-        <f t="shared" si="1"/>
-        <v>56</v>
-      </c>
-      <c r="L19" s="51">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="51">
-        <f t="shared" si="1"/>
+      <c r="D21" s="51">
+        <f>+D19+D18+D17+D16+D15+D14+D13+D12+D11+D10+D9+D8+D7+D6+D4+D5</f>
+        <v>200</v>
+      </c>
+      <c r="E21" s="51">
+        <f>+E19+E18+E17+E16+E15+E14+E13+E12+E11+E10+E9+E8+E7+E6+E4+E5</f>
+        <v>200</v>
+      </c>
+      <c r="F21" s="51">
+        <f>+F19+F18+F17+F16+F15+F14+F13+F12+F11+F10+F9+F8+F7+F6+F4+F5</f>
+        <v>166</v>
+      </c>
+      <c r="G21" s="51">
+        <f>+G19+G18+G17+G16+G15+G14+G13+G12+G11+G10+G9+G8+G7+G6+G4+G5</f>
+        <v>154</v>
+      </c>
+      <c r="H21" s="51">
+        <f>+H19+H18+H17+H16+H15+H14+H13+H12+H11+H10+H9+H8+H7+H6+H4+H5</f>
+        <v>154</v>
+      </c>
+      <c r="I21" s="51">
+        <f>+I19+I18+I17+I16+I15+I14+I13+I12+I11+I10+I9+I8+I7+I6+I4+I5</f>
+        <v>114</v>
+      </c>
+      <c r="J21" s="51">
+        <f>+J19+J18+J17+J16+J15+J14+J13+J12+J11+J10+J9+J8+J7+J6+J4+J5</f>
+        <v>114</v>
+      </c>
+      <c r="K21" s="51">
+        <f>+K19+K18+K17+K16+K15+K14+K13+K12+K11+K10+K9+K8+K7+K6+K4+K5</f>
+        <v>89</v>
+      </c>
+      <c r="L21" s="51">
+        <f>+L19+L18+L17+L16+L15+L14+L13+L12+L11+L10+L9+L8+L7+L6+L4+L5</f>
+        <v>61</v>
+      </c>
+      <c r="M21" s="51">
+        <f>+M19+M18+M17+M16+M15+M14+M13+M12+M11+M10+M9+M8+M7+M6+M4+M5</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>